<commit_message>
actualizacion de nota standar
</commit_message>
<xml_diff>
--- a/BBDD Gran Concepcion.xlsx
+++ b/BBDD Gran Concepcion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\benja\PP\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224CD0E1-5E32-45DB-B10A-C0B98464A094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B0AFB6-F67F-4664-B71E-92D8D93080D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -760,7 +760,9 @@
       <c r="AB2" s="2"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
       <c r="B3" s="6" t="s">
         <v>32</v>
       </c>
@@ -784,7 +786,9 @@
       <c r="R3" s="10"/>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
@@ -808,7 +812,9 @@
       <c r="R4" s="10"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
       <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
@@ -832,7 +838,9 @@
       <c r="R5" s="10"/>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
       <c r="B6" s="6" t="s">
         <v>35</v>
       </c>
@@ -856,7 +864,9 @@
       <c r="R6" s="10"/>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
       <c r="B7" s="11" t="s">
         <v>38</v>
       </c>
@@ -880,7 +890,9 @@
       <c r="R7" s="10"/>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
       <c r="B8" s="11" t="s">
         <v>38</v>
       </c>
@@ -904,7 +916,9 @@
       <c r="R8" s="10"/>
     </row>
     <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
       <c r="B9" s="11" t="s">
         <v>41</v>
       </c>
@@ -928,7 +942,9 @@
       <c r="R9" s="10"/>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
       <c r="B10" s="11" t="s">
         <v>41</v>
       </c>
@@ -952,7 +968,9 @@
       <c r="R10" s="10"/>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
       <c r="B11" s="11" t="s">
         <v>41</v>
       </c>
@@ -976,7 +994,9 @@
       <c r="R11" s="10"/>
     </row>
     <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
       <c r="B12" s="11" t="s">
         <v>41</v>
       </c>
@@ -1000,7 +1020,9 @@
       <c r="R12" s="10"/>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="10">
+        <v>11</v>
+      </c>
       <c r="B13" s="11" t="s">
         <v>46</v>
       </c>
@@ -1024,7 +1046,9 @@
       <c r="R13" s="10"/>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
       <c r="B14" s="11" t="s">
         <v>46</v>
       </c>
@@ -1048,7 +1072,9 @@
       <c r="R14" s="10"/>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="10">
+        <v>13</v>
+      </c>
       <c r="B15" s="11" t="s">
         <v>46</v>
       </c>
@@ -1072,7 +1098,9 @@
       <c r="R15" s="10"/>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="10">
+        <v>14</v>
+      </c>
       <c r="B16" s="11" t="s">
         <v>46</v>
       </c>
@@ -1096,7 +1124,9 @@
       <c r="R16" s="10"/>
     </row>
     <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="10">
+        <v>15</v>
+      </c>
       <c r="B17" s="11" t="s">
         <v>46</v>
       </c>
@@ -1120,7 +1150,9 @@
       <c r="R17" s="10"/>
     </row>
     <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="10">
+        <v>16</v>
+      </c>
       <c r="B18" s="11" t="s">
         <v>46</v>
       </c>
@@ -1144,7 +1176,9 @@
       <c r="R18" s="10"/>
     </row>
     <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="10">
+        <v>17</v>
+      </c>
       <c r="B19" s="11" t="s">
         <v>46</v>
       </c>
@@ -1168,7 +1202,9 @@
       <c r="R19" s="10"/>
     </row>
     <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
+      <c r="A20" s="10">
+        <v>18</v>
+      </c>
       <c r="B20" s="11" t="s">
         <v>46</v>
       </c>
@@ -1192,7 +1228,9 @@
       <c r="R20" s="10"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
+      <c r="A21" s="10">
+        <v>19</v>
+      </c>
       <c r="B21" s="11" t="s">
         <v>46</v>
       </c>
@@ -1216,7 +1254,9 @@
       <c r="R21" s="10"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
+      <c r="A22" s="10">
+        <v>20</v>
+      </c>
       <c r="B22" s="11" t="s">
         <v>46</v>
       </c>
@@ -1240,7 +1280,9 @@
       <c r="R22" s="10"/>
     </row>
     <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
+      <c r="A23" s="10">
+        <v>21</v>
+      </c>
       <c r="B23" s="11" t="s">
         <v>46</v>
       </c>
@@ -1264,7 +1306,9 @@
       <c r="R23" s="10"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+      <c r="A24" s="10">
+        <v>22</v>
+      </c>
       <c r="B24" s="11" t="s">
         <v>58</v>
       </c>
@@ -1288,7 +1332,9 @@
       <c r="R24" s="10"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
+      <c r="A25" s="10">
+        <v>23</v>
+      </c>
       <c r="B25" s="11" t="s">
         <v>58</v>
       </c>
@@ -1312,7 +1358,9 @@
       <c r="R25" s="10"/>
     </row>
     <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="10">
+        <v>24</v>
+      </c>
       <c r="B26" s="11" t="s">
         <v>58</v>
       </c>
@@ -1336,7 +1384,9 @@
       <c r="R26" s="10"/>
     </row>
     <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+      <c r="A27" s="10">
+        <v>25</v>
+      </c>
       <c r="B27" s="11" t="s">
         <v>58</v>
       </c>
@@ -1360,7 +1410,9 @@
       <c r="R27" s="10"/>
     </row>
     <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
+      <c r="A28" s="10">
+        <v>26</v>
+      </c>
       <c r="B28" s="11" t="s">
         <v>63</v>
       </c>
@@ -1384,7 +1436,9 @@
       <c r="R28" s="10"/>
     </row>
     <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
+      <c r="A29" s="10">
+        <v>27</v>
+      </c>
       <c r="B29" s="11" t="s">
         <v>63</v>
       </c>
@@ -1408,7 +1462,9 @@
       <c r="R29" s="10"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
+      <c r="A30" s="10">
+        <v>28</v>
+      </c>
       <c r="B30" s="11" t="s">
         <v>63</v>
       </c>
@@ -1432,7 +1488,9 @@
       <c r="R30" s="10"/>
     </row>
     <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
+      <c r="A31" s="10">
+        <v>29</v>
+      </c>
       <c r="B31" s="11" t="s">
         <v>63</v>
       </c>
@@ -1456,7 +1514,9 @@
       <c r="R31" s="10"/>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
+      <c r="A32" s="10">
+        <v>30</v>
+      </c>
       <c r="B32" s="11" t="s">
         <v>68</v>
       </c>
@@ -1480,7 +1540,9 @@
       <c r="R32" s="10"/>
     </row>
     <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
+      <c r="A33" s="10">
+        <v>31</v>
+      </c>
       <c r="B33" s="11" t="s">
         <v>70</v>
       </c>
@@ -1504,7 +1566,9 @@
       <c r="R33" s="10"/>
     </row>
     <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+      <c r="A34" s="10">
+        <v>32</v>
+      </c>
       <c r="B34" s="11" t="s">
         <v>70</v>
       </c>
@@ -1528,7 +1592,9 @@
       <c r="R34" s="10"/>
     </row>
     <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
+      <c r="A35" s="10">
+        <v>33</v>
+      </c>
       <c r="B35" s="11" t="s">
         <v>73</v>
       </c>
@@ -1552,7 +1618,9 @@
       <c r="R35" s="10"/>
     </row>
     <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
+      <c r="A36" s="10">
+        <v>34</v>
+      </c>
       <c r="B36" s="11" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
edición pobladoras wallpen y h Rocuant
</commit_message>
<xml_diff>
--- a/BBDD Gran Concepcion.xlsx
+++ b/BBDD Gran Concepcion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\benja\PP\datos conce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DDFC89-4E73-454C-8889-B1B7BB794328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A99E53B-AFA3-422D-9069-850DDC48167D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
   <si>
     <t>FOLIO</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>Comité de Cesantes Hualpen</t>
+  </si>
+  <si>
+    <t>Bloque Mujeres Nonguenche</t>
+  </si>
+  <si>
+    <t>Asamblea Barrial Puchacay</t>
   </si>
 </sst>
 </file>
@@ -649,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB1028"/>
+  <dimension ref="A1:AB1030"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1393,10 +1399,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>59</v>
+        <v>46</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -1419,10 +1425,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -1448,7 +1454,7 @@
         <v>58</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -1473,8 +1479,8 @@
       <c r="B29" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>62</v>
+      <c r="C29" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -1499,8 +1505,8 @@
       <c r="B30" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>79</v>
+      <c r="C30" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -1525,8 +1531,8 @@
       <c r="B31" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>81</v>
+      <c r="C31" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -1549,10 +1555,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -1575,10 +1581,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -1604,7 +1610,7 @@
         <v>63</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -1630,7 +1636,7 @@
         <v>63</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -1653,10 +1659,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
@@ -1679,10 +1685,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
@@ -1705,10 +1711,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
@@ -1731,10 +1737,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -1757,10 +1763,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -1783,10 +1789,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -1808,12 +1814,62 @@
       <c r="A42" s="10">
         <v>40</v>
       </c>
+      <c r="B42" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
     </row>
     <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-    </row>
-    <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="A43" s="10">
+        <v>41</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+    </row>
+    <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+    </row>
     <row r="46" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2797,6 +2853,8 @@
     <row r="1026" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1027" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1028" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1029" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1030" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:H1"/>

</xml_diff>

<commit_message>
agregue imag y modifique md
</commit_message>
<xml_diff>
--- a/BBDD Gran Concepcion.xlsx
+++ b/BBDD Gran Concepcion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\benja\PP\datos conce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A99E53B-AFA3-422D-9069-850DDC48167D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049DE15C-AC17-492F-A6AB-80E289C780BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
   <si>
     <t>FOLIO</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>Asamblea Barrial Puchacay</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Red Abastecimiento Hualpencillo</t>
   </si>
 </sst>
 </file>
@@ -655,75 +661,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB1030"/>
+  <dimension ref="A1:AC1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="3" width="31.77734375" customWidth="1"/>
-    <col min="4" max="5" width="25.77734375" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
-    <col min="7" max="17" width="25.77734375" customWidth="1"/>
-    <col min="18" max="18" width="73.6640625" customWidth="1"/>
-    <col min="19" max="28" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="4" width="31.77734375" customWidth="1"/>
+    <col min="5" max="6" width="25.77734375" customWidth="1"/>
+    <col min="7" max="7" width="26.77734375" customWidth="1"/>
+    <col min="8" max="18" width="25.77734375" customWidth="1"/>
+    <col min="19" max="19" width="73.6640625" customWidth="1"/>
+    <col min="20" max="29" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -733,59 +741,59 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
-    </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="AC1" s="1"/>
+    </row>
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
@@ -795,18 +803,21 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
-    </row>
-    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="AC2" s="2"/>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -821,18 +832,21 @@
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
-    </row>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="S3" s="10"/>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="10">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -847,18 +861,21 @@
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
-    </row>
-    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="S4" s="10"/>
+    </row>
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -873,18 +890,21 @@
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
-    </row>
-    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="S5" s="10"/>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="10">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -899,18 +919,21 @@
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
-    </row>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="S6" s="10"/>
+    </row>
+    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -925,18 +948,21 @@
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
-    </row>
-    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="S7" s="10"/>
+    </row>
+    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10">
+        <v>2</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -951,18 +977,21 @@
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
-    </row>
-    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="S8" s="10"/>
+    </row>
+    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -977,18 +1006,21 @@
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
-    </row>
-    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="S9" s="10"/>
+    </row>
+    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -1003,18 +1035,21 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
-    </row>
-    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="S10" s="10"/>
+    </row>
+    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10">
+        <v>3</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -1029,18 +1064,21 @@
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
-    </row>
-    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="S11" s="10"/>
+    </row>
+    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10">
+        <v>4</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1055,18 +1093,21 @@
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
-    </row>
-    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="S12" s="10"/>
+    </row>
+    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10">
+        <v>5</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1081,18 +1122,21 @@
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
-    </row>
-    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="S13" s="10"/>
+    </row>
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10">
+        <v>6</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="D14" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -1107,18 +1151,21 @@
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
-    </row>
-    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="S14" s="10"/>
+    </row>
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10">
+        <v>1</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -1133,18 +1180,21 @@
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
-    </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="S15" s="10"/>
+    </row>
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -1159,18 +1209,21 @@
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
-    </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="S16" s="10"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10">
+        <v>3</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -1185,18 +1238,21 @@
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
-    </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="S17" s="10"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10">
+        <v>4</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -1211,18 +1267,21 @@
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
-    </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="S18" s="10"/>
+    </row>
+    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10">
+        <v>5</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
@@ -1237,18 +1296,21 @@
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
-    </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="S19" s="10"/>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10">
+        <v>6</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -1263,18 +1325,21 @@
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
-    </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="S20" s="10"/>
+    </row>
+    <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10">
+        <v>7</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -1289,18 +1354,21 @@
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
-    </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+      <c r="S21" s="10"/>
+    </row>
+    <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10">
+        <v>8</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -1315,18 +1383,21 @@
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
-    </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+      <c r="S22" s="10"/>
+    </row>
+    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10">
+        <v>9</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -1341,18 +1412,21 @@
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
-    </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="S23" s="10"/>
+    </row>
+    <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="10">
+        <v>10</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
@@ -1367,18 +1441,21 @@
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
-    </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="S24" s="10"/>
+    </row>
+    <row r="25" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10">
+        <v>11</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -1393,18 +1470,21 @@
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
-    </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="S25" s="10"/>
+    </row>
+    <row r="26" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10">
+        <v>12</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="D26" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -1419,18 +1499,21 @@
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
-    </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="S26" s="10"/>
+    </row>
+    <row r="27" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10">
+        <v>13</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="D27" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -1445,18 +1528,21 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
-    </row>
-    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="S27" s="10"/>
+    </row>
+    <row r="28" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -1471,18 +1557,21 @@
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
-    </row>
-    <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+      <c r="S28" s="10"/>
+    </row>
+    <row r="29" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10">
+        <v>2</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="D29" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -1497,18 +1586,21 @@
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
-    </row>
-    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+      <c r="S29" s="10"/>
+    </row>
+    <row r="30" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="10">
+        <v>3</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D30" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -1523,18 +1615,21 @@
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
-    </row>
-    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
+      <c r="S30" s="10"/>
+    </row>
+    <row r="31" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10">
+        <v>4</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -1549,18 +1644,21 @@
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
       <c r="R31" s="10"/>
-    </row>
-    <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+      <c r="S31" s="10"/>
+    </row>
+    <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="10">
+        <v>5</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
@@ -1575,18 +1673,21 @@
       <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
       <c r="R32" s="10"/>
-    </row>
-    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+      <c r="S32" s="10"/>
+    </row>
+    <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="10">
+        <v>6</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="D33" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -1601,18 +1702,21 @@
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
       <c r="R33" s="10"/>
-    </row>
-    <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
+      <c r="S33" s="10"/>
+    </row>
+    <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="10"/>
+      <c r="B34" s="10">
+        <v>7</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>85</v>
+      </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
@@ -1627,18 +1731,21 @@
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
-    </row>
-    <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
+      <c r="S34" s="10"/>
+    </row>
+    <row r="35" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10">
+        <v>1</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="10"/>
+      <c r="D35" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -1653,18 +1760,21 @@
       <c r="P35" s="10"/>
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
-    </row>
-    <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
+      <c r="S35" s="10"/>
+    </row>
+    <row r="36" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10">
+        <v>2</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" s="10"/>
+      <c r="D36" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -1679,18 +1789,21 @@
       <c r="P36" s="10"/>
       <c r="Q36" s="10"/>
       <c r="R36" s="10"/>
-    </row>
-    <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+      <c r="S36" s="10"/>
+    </row>
+    <row r="37" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10">
+        <v>3</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="10"/>
+      <c r="D37" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -1705,18 +1818,21 @@
       <c r="P37" s="10"/>
       <c r="Q37" s="10"/>
       <c r="R37" s="10"/>
-    </row>
-    <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
+      <c r="S37" s="10"/>
+    </row>
+    <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38" s="10"/>
+      <c r="B38" s="10">
+        <v>4</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -1731,18 +1847,21 @@
       <c r="P38" s="10"/>
       <c r="Q38" s="10"/>
       <c r="R38" s="10"/>
-    </row>
-    <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10">
+      <c r="S38" s="10"/>
+    </row>
+    <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="10"/>
+      <c r="B39" s="10">
+        <v>1</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -1757,18 +1876,21 @@
       <c r="P39" s="10"/>
       <c r="Q39" s="10"/>
       <c r="R39" s="10"/>
-    </row>
-    <row r="40" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
+      <c r="S39" s="10"/>
+    </row>
+    <row r="40" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10">
+        <v>1</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="10"/>
+      <c r="D40" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
@@ -1783,18 +1905,21 @@
       <c r="P40" s="10"/>
       <c r="Q40" s="10"/>
       <c r="R40" s="10"/>
-    </row>
-    <row r="41" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10">
+      <c r="S40" s="10"/>
+    </row>
+    <row r="41" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D41" s="10"/>
+      <c r="B41" s="10">
+        <v>2</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -1809,18 +1934,21 @@
       <c r="P41" s="10"/>
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
-    </row>
-    <row r="42" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10">
+      <c r="S41" s="10"/>
+    </row>
+    <row r="42" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10">
+        <v>1</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="10"/>
+      <c r="D42" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
@@ -1835,18 +1963,21 @@
       <c r="P42" s="10"/>
       <c r="Q42" s="10"/>
       <c r="R42" s="10"/>
-    </row>
-    <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10">
+      <c r="S42" s="10"/>
+    </row>
+    <row r="43" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="10"/>
+      <c r="B43" s="10">
+        <v>2</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>77</v>
+      </c>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
@@ -1861,18 +1992,45 @@
       <c r="P43" s="10"/>
       <c r="Q43" s="10"/>
       <c r="R43" s="10"/>
-    </row>
-    <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-    </row>
-    <row r="46" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="S43" s="10"/>
+    </row>
+    <row r="44" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" s="10">
+        <v>1</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10"/>
+    </row>
+    <row r="45" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="10"/>
+    </row>
+    <row r="46" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="7"/>
+    </row>
+    <row r="47" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2855,9 +3013,10 @@
     <row r="1028" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1029" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1030" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1031" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
agregue imagenes y modifique notas
</commit_message>
<xml_diff>
--- a/BBDD Gran Concepcion.xlsx
+++ b/BBDD Gran Concepcion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\benja\PP\datos conce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049DE15C-AC17-492F-A6AB-80E289C780BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23110D3B-8DAD-4FC5-974F-E618722C2973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -663,7 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nueda edición, se adjuntaron categorias totales
</commit_message>
<xml_diff>
--- a/BBDD Gran Concepcion.xlsx
+++ b/BBDD Gran Concepcion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\benja\PP\datos conce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5D7393-D262-480A-A368-BB7C1754BB9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528EA64F-29D8-4EDC-827A-C5D293C45D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1032"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>